<commit_message>
actual vs predicted done
</commit_message>
<xml_diff>
--- a/Austrailian working/RMSE table.xlsx
+++ b/Austrailian working/RMSE table.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dev\Time Series Forcasting (RBL)\Austrailian working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435C35A1-5E7C-4E47-ACEA-A9AE0AAE28C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEF3357-AD56-4F5F-84BB-1BFA5312D541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15930" xr2:uid="{2D132367-4F74-4C4C-BC78-BD381818FE0F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Bin ID</t>
   </si>
@@ -54,28 +54,16 @@
     <t>SARIMA</t>
   </si>
   <si>
-    <t>Comparing last week actual to last week predicted</t>
-  </si>
-  <si>
     <t>Comparing last week actual to new week predicted</t>
   </si>
   <si>
-    <t>ToDO</t>
-  </si>
-  <si>
-    <t>Identify low medium and High</t>
-  </si>
-  <si>
-    <t>Graph for both tables for each bin</t>
-  </si>
-  <si>
-    <t>Hybridization</t>
-  </si>
-  <si>
-    <t>Exponential Smoothing X LSTM</t>
-  </si>
-  <si>
-    <t>Avergage for hybridization</t>
+    <t>1510830 (Low)</t>
+  </si>
+  <si>
+    <t>1511208(High)</t>
+  </si>
+  <si>
+    <t>1511196(Med)</t>
   </si>
 </sst>
 </file>
@@ -106,7 +94,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,15 +139,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,232 +465,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FD82B5-49D8-462A-8FFB-65BF83901755}">
-  <dimension ref="B1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C53688-D561-4517-A682-7A5B3DD58E49}">
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1510830</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1511191</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1511194</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.90368099999999996</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.27706599999999998</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.86543400000000004</v>
-      </c>
-      <c r="F4" s="6">
-        <f>SUM(C4,D4,E4)/3</f>
-        <v>0.68206033333333327</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1.083456</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.063256</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.90451499999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
+        <v>1.0538572213581501</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.94996996612788198</v>
+      </c>
+      <c r="E6" s="2">
         <v>1.06853623249979</v>
       </c>
-      <c r="D5" s="2">
-        <v>8.8817841000000008</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.74695407416473103</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" ref="F5:F7" si="0">SUM(C5,D5,E5)/3</f>
-        <v>3.5657581355548409</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
+        <v>1.0665865421101299</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.99343867448644896</v>
+      </c>
+      <c r="E7" s="2">
         <v>0.90728084462780201</v>
       </c>
-      <c r="D6" s="2">
-        <v>5.1184474524927297E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.74288964641022004</v>
-      </c>
-      <c r="F6" s="6">
-        <f t="shared" si="0"/>
-        <v>0.56711832185431643</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1510830</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1511191</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1511194</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <f>SUM(C13,D13,E13)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <f t="shared" ref="F14:F16" si="1">SUM(C14,D14,E14)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C8" s="2">
+        <v>1.04503985259496</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0951377350609099</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.00153931735747</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B1:F1"/>
+  <mergeCells count="4">
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>